<commit_message>
modificacoes tela index.html, variaveis,css cor tema formulario, script-horimetro.js settimeout fetch
</commit_message>
<xml_diff>
--- a/backend/planilhas/banco-de-dados-horimetro.xlsx
+++ b/backend/planilhas/banco-de-dados-horimetro.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1732,9 +1732,161 @@
         <v>teste de lançamento de horimetro</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B36" t="str">
+        <v>17/06/2025, 16:35</v>
+      </c>
+      <c r="C36" t="str">
+        <v>VJ3WQ</v>
+      </c>
+      <c r="D36" t="str">
+        <v>2025-06-17</v>
+      </c>
+      <c r="E36" t="str">
+        <v>25</v>
+      </c>
+      <c r="F36" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G36" t="str">
+        <v>100</v>
+      </c>
+      <c r="H36" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I36" t="str">
+        <v>328</v>
+      </c>
+      <c r="J36" t="str">
+        <v>341</v>
+      </c>
+      <c r="K36" t="str">
+        <v>13.0</v>
+      </c>
+      <c r="L36" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B37" t="str">
+        <v>17/06/2025, 16:50</v>
+      </c>
+      <c r="C37" t="str">
+        <v>SMHCV</v>
+      </c>
+      <c r="D37" t="str">
+        <v>2025-06-17</v>
+      </c>
+      <c r="E37" t="str">
+        <v>25</v>
+      </c>
+      <c r="F37" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G37" t="str">
+        <v>100</v>
+      </c>
+      <c r="H37" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I37" t="str">
+        <v>341</v>
+      </c>
+      <c r="J37" t="str">
+        <v>352</v>
+      </c>
+      <c r="K37" t="str">
+        <v>11.0</v>
+      </c>
+      <c r="L37" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B38" t="str">
+        <v>17/06/2025, 16:51</v>
+      </c>
+      <c r="C38" t="str">
+        <v>27AT8</v>
+      </c>
+      <c r="D38" t="str">
+        <v>2025-06-17</v>
+      </c>
+      <c r="E38" t="str">
+        <v>55</v>
+      </c>
+      <c r="F38" t="str">
+        <v>1/2-PIVO</v>
+      </c>
+      <c r="G38" t="str">
+        <v>100</v>
+      </c>
+      <c r="H38" t="str">
+        <v>6.48</v>
+      </c>
+      <c r="I38" t="str">
+        <v>875</v>
+      </c>
+      <c r="J38" t="str">
+        <v>883.8</v>
+      </c>
+      <c r="K38" t="str">
+        <v>8.8</v>
+      </c>
+      <c r="L38" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B39" t="str">
+        <v>17/06/2025, 16:56</v>
+      </c>
+      <c r="C39" t="str">
+        <v>T04U7</v>
+      </c>
+      <c r="D39" t="str">
+        <v>2025-06-17</v>
+      </c>
+      <c r="E39" t="str">
+        <v>25</v>
+      </c>
+      <c r="F39" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G39" t="str">
+        <v>12</v>
+      </c>
+      <c r="H39" t="str">
+        <v>48.33</v>
+      </c>
+      <c r="I39" t="str">
+        <v>352</v>
+      </c>
+      <c r="J39" t="str">
+        <v>363</v>
+      </c>
+      <c r="K39" t="str">
+        <v>11.0</v>
+      </c>
+      <c r="L39" t="str">
+        <v>sdsdsds dsds</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L35"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L39"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modificacoes 18-09-26, add ultimaData, construcao relogio na cabecalho
</commit_message>
<xml_diff>
--- a/backend/planilhas/banco-de-dados-horimetro.xlsx
+++ b/backend/planilhas/banco-de-dados-horimetro.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:L78"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1884,9 +1884,1491 @@
         <v>sdsdsds dsds</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B40" t="str">
+        <v>17/06/2025, 18:30</v>
+      </c>
+      <c r="C40" t="str">
+        <v>7V3WV</v>
+      </c>
+      <c r="D40" t="str">
+        <v>2025-06-17</v>
+      </c>
+      <c r="E40" t="str">
+        <v>25</v>
+      </c>
+      <c r="F40" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G40" t="str">
+        <v>100</v>
+      </c>
+      <c r="H40" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I40" t="str">
+        <v>363</v>
+      </c>
+      <c r="J40" t="str">
+        <v>375</v>
+      </c>
+      <c r="K40" t="str">
+        <v>12.0</v>
+      </c>
+      <c r="L40" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B41" t="str">
+        <v>17/06/2025, 18:31</v>
+      </c>
+      <c r="C41" t="str">
+        <v>4YZCP</v>
+      </c>
+      <c r="D41" t="str">
+        <v>2025-06-17</v>
+      </c>
+      <c r="E41" t="str">
+        <v>58</v>
+      </c>
+      <c r="F41" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G41" t="str">
+        <v>100</v>
+      </c>
+      <c r="H41" t="str">
+        <v>6.54</v>
+      </c>
+      <c r="I41" t="str">
+        <v>250</v>
+      </c>
+      <c r="J41" t="str">
+        <v>265</v>
+      </c>
+      <c r="K41" t="str">
+        <v>15.0</v>
+      </c>
+      <c r="L41" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B42" t="str">
+        <v>17/06/2025, 18:31</v>
+      </c>
+      <c r="C42" t="str">
+        <v>Y4FZA</v>
+      </c>
+      <c r="D42" t="str">
+        <v>2025-06-18</v>
+      </c>
+      <c r="E42" t="str">
+        <v>25</v>
+      </c>
+      <c r="F42" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G42" t="str">
+        <v>100</v>
+      </c>
+      <c r="H42" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I42" t="str">
+        <v>375</v>
+      </c>
+      <c r="J42" t="str">
+        <v>387</v>
+      </c>
+      <c r="K42" t="str">
+        <v>12.0</v>
+      </c>
+      <c r="L42" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B43" t="str">
+        <v>17/06/2025, 18:41</v>
+      </c>
+      <c r="C43" t="str">
+        <v>ZGYT6</v>
+      </c>
+      <c r="D43" t="str">
+        <v>2025-06-17</v>
+      </c>
+      <c r="E43" t="str">
+        <v>25</v>
+      </c>
+      <c r="F43" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G43" t="str">
+        <v>25</v>
+      </c>
+      <c r="H43" t="str">
+        <v>23.20</v>
+      </c>
+      <c r="I43" t="str">
+        <v>387</v>
+      </c>
+      <c r="J43" t="str">
+        <v>400</v>
+      </c>
+      <c r="K43" t="str">
+        <v>13.0</v>
+      </c>
+      <c r="L43" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B44" t="str">
+        <v>17/06/2025, 18:42</v>
+      </c>
+      <c r="C44" t="str">
+        <v>F40RK</v>
+      </c>
+      <c r="D44" t="str">
+        <v>2025-06-10</v>
+      </c>
+      <c r="E44" t="str">
+        <v>48</v>
+      </c>
+      <c r="F44" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G44" t="str">
+        <v>70</v>
+      </c>
+      <c r="H44" t="str">
+        <v>9.71</v>
+      </c>
+      <c r="I44" t="str">
+        <v>280.2</v>
+      </c>
+      <c r="J44" t="str">
+        <v>303.5</v>
+      </c>
+      <c r="K44" t="str">
+        <v>23.3</v>
+      </c>
+      <c r="L44" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B45" t="str">
+        <v>17/06/2025, 18:42</v>
+      </c>
+      <c r="C45" t="str">
+        <v>T6O5H</v>
+      </c>
+      <c r="D45" t="str">
+        <v>2025-06-17</v>
+      </c>
+      <c r="E45" t="str">
+        <v>43</v>
+      </c>
+      <c r="F45" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G45" t="str">
+        <v>100</v>
+      </c>
+      <c r="H45" t="str">
+        <v>6.79</v>
+      </c>
+      <c r="I45" t="str">
+        <v>0</v>
+      </c>
+      <c r="J45" t="str">
+        <v>15</v>
+      </c>
+      <c r="K45" t="str">
+        <v>15.0</v>
+      </c>
+      <c r="L45" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B46" t="str">
+        <v>17/06/2025, 18:45</v>
+      </c>
+      <c r="C46" t="str">
+        <v>B8KS2</v>
+      </c>
+      <c r="D46" t="str">
+        <v>2025-06-17</v>
+      </c>
+      <c r="E46" t="str">
+        <v>25</v>
+      </c>
+      <c r="F46" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G46" t="str">
+        <v>100</v>
+      </c>
+      <c r="H46" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I46" t="str">
+        <v>400</v>
+      </c>
+      <c r="J46" t="str">
+        <v>412</v>
+      </c>
+      <c r="K46" t="str">
+        <v>12.0</v>
+      </c>
+      <c r="L46" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B47" t="str">
+        <v>17/06/2025, 18:46</v>
+      </c>
+      <c r="C47" t="str">
+        <v>56F5V</v>
+      </c>
+      <c r="D47" t="str">
+        <v>2025-06-18</v>
+      </c>
+      <c r="E47" t="str">
+        <v>25</v>
+      </c>
+      <c r="F47" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G47" t="str">
+        <v>100</v>
+      </c>
+      <c r="H47" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I47" t="str">
+        <v>412</v>
+      </c>
+      <c r="J47" t="str">
+        <v>425</v>
+      </c>
+      <c r="K47" t="str">
+        <v>13.0</v>
+      </c>
+      <c r="L47" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B48" t="str">
+        <v>17/06/2025, 18:56</v>
+      </c>
+      <c r="C48" t="str">
+        <v>B5Q45</v>
+      </c>
+      <c r="D48" t="str">
+        <v>2025-06-16</v>
+      </c>
+      <c r="E48" t="str">
+        <v>25</v>
+      </c>
+      <c r="F48" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G48" t="str">
+        <v>100</v>
+      </c>
+      <c r="H48" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I48" t="str">
+        <v>425</v>
+      </c>
+      <c r="J48" t="str">
+        <v>437</v>
+      </c>
+      <c r="K48" t="str">
+        <v>12.0</v>
+      </c>
+      <c r="L48" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B49" t="str">
+        <v>17/06/2025, 19:05</v>
+      </c>
+      <c r="C49" t="str">
+        <v>ESG48</v>
+      </c>
+      <c r="D49" t="str">
+        <v>2025-06-18</v>
+      </c>
+      <c r="E49" t="str">
+        <v>25</v>
+      </c>
+      <c r="F49" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G49" t="str">
+        <v>100</v>
+      </c>
+      <c r="H49" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I49" t="str">
+        <v>437</v>
+      </c>
+      <c r="J49" t="str">
+        <v>449</v>
+      </c>
+      <c r="K49" t="str">
+        <v>12.0</v>
+      </c>
+      <c r="L49" t="str">
+        <v>teste de reste inputs</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B50" t="str">
+        <v>17/06/2025, 19:20</v>
+      </c>
+      <c r="C50" t="str">
+        <v>E7NP4</v>
+      </c>
+      <c r="D50" t="str">
+        <v>2025-06-17</v>
+      </c>
+      <c r="E50" t="str">
+        <v>25</v>
+      </c>
+      <c r="F50" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G50" t="str">
+        <v>100</v>
+      </c>
+      <c r="H50" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I50" t="str">
+        <v>449</v>
+      </c>
+      <c r="J50" t="str">
+        <v>462</v>
+      </c>
+      <c r="K50" t="str">
+        <v>13.0</v>
+      </c>
+      <c r="L50" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B51" t="str">
+        <v>17/06/2025, 19:20</v>
+      </c>
+      <c r="C51" t="str">
+        <v>1IFES</v>
+      </c>
+      <c r="D51" t="str">
+        <v>2025-06-24</v>
+      </c>
+      <c r="E51" t="str">
+        <v>25</v>
+      </c>
+      <c r="F51" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G51" t="str">
+        <v>100</v>
+      </c>
+      <c r="H51" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I51" t="str">
+        <v>462</v>
+      </c>
+      <c r="J51" t="str">
+        <v>475</v>
+      </c>
+      <c r="K51" t="str">
+        <v>13.0</v>
+      </c>
+      <c r="L51" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B52" t="str">
+        <v>17/06/2025, 19:26</v>
+      </c>
+      <c r="C52" t="str">
+        <v>S23A8</v>
+      </c>
+      <c r="D52" t="str">
+        <v>2025-06-18</v>
+      </c>
+      <c r="E52" t="str">
+        <v>25</v>
+      </c>
+      <c r="F52" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G52" t="str">
+        <v>100</v>
+      </c>
+      <c r="H52" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I52" t="str">
+        <v>475</v>
+      </c>
+      <c r="J52" t="str">
+        <v>488</v>
+      </c>
+      <c r="K52" t="str">
+        <v>13.0</v>
+      </c>
+      <c r="L52" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B53" t="str">
+        <v>17/06/2025, 19:27</v>
+      </c>
+      <c r="C53" t="str">
+        <v>AHIEI</v>
+      </c>
+      <c r="D53" t="str">
+        <v>2025-06-18</v>
+      </c>
+      <c r="E53" t="str">
+        <v>48</v>
+      </c>
+      <c r="F53" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G53" t="str">
+        <v>70</v>
+      </c>
+      <c r="H53" t="str">
+        <v>9.71</v>
+      </c>
+      <c r="I53" t="str">
+        <v>303.5</v>
+      </c>
+      <c r="J53" t="str">
+        <v>326</v>
+      </c>
+      <c r="K53" t="str">
+        <v>22.5</v>
+      </c>
+      <c r="L53" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B54" t="str">
+        <v>17/06/2025, 19:29</v>
+      </c>
+      <c r="C54" t="str">
+        <v>MCVJL</v>
+      </c>
+      <c r="D54" t="str">
+        <v>2025-06-16</v>
+      </c>
+      <c r="E54" t="str">
+        <v>47</v>
+      </c>
+      <c r="F54" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G54" t="str">
+        <v>100</v>
+      </c>
+      <c r="H54" t="str">
+        <v>7.42</v>
+      </c>
+      <c r="I54" t="str">
+        <v>0</v>
+      </c>
+      <c r="J54" t="str">
+        <v>15</v>
+      </c>
+      <c r="K54" t="str">
+        <v>15.0</v>
+      </c>
+      <c r="L54" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B55" t="str">
+        <v>17/06/2025, 19:29</v>
+      </c>
+      <c r="C55" t="str">
+        <v>P9HE8</v>
+      </c>
+      <c r="D55" t="str">
+        <v>2025-06-24</v>
+      </c>
+      <c r="E55" t="str">
+        <v>70</v>
+      </c>
+      <c r="F55" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G55" t="str">
+        <v>100</v>
+      </c>
+      <c r="H55" t="str">
+        <v>6.42</v>
+      </c>
+      <c r="I55" t="str">
+        <v>0</v>
+      </c>
+      <c r="J55" t="str">
+        <v>15</v>
+      </c>
+      <c r="K55" t="str">
+        <v>15.0</v>
+      </c>
+      <c r="L55" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B56" t="str">
+        <v>17/06/2025, 19:31</v>
+      </c>
+      <c r="C56" t="str">
+        <v>K7E85</v>
+      </c>
+      <c r="D56" t="str">
+        <v>2025-06-18</v>
+      </c>
+      <c r="E56" t="str">
+        <v>25</v>
+      </c>
+      <c r="F56" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G56" t="str">
+        <v>100</v>
+      </c>
+      <c r="H56" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I56" t="str">
+        <v>488</v>
+      </c>
+      <c r="J56" t="str">
+        <v>500</v>
+      </c>
+      <c r="K56" t="str">
+        <v>12.0</v>
+      </c>
+      <c r="L56" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B57" t="str">
+        <v>18/06/2025, 00:37</v>
+      </c>
+      <c r="C57" t="str">
+        <v>1EHEW</v>
+      </c>
+      <c r="D57" t="str">
+        <v>2025-06-18</v>
+      </c>
+      <c r="E57" t="str">
+        <v>10</v>
+      </c>
+      <c r="F57" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G57" t="str">
+        <v>100</v>
+      </c>
+      <c r="H57" t="str">
+        <v>6.30</v>
+      </c>
+      <c r="I57" t="str">
+        <v>189</v>
+      </c>
+      <c r="J57" t="str">
+        <v>204</v>
+      </c>
+      <c r="K57" t="str">
+        <v>15.0</v>
+      </c>
+      <c r="L57" t="str">
+        <v>fertirrigação</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B58" t="str">
+        <v>18/06/2025, 01:38</v>
+      </c>
+      <c r="C58" t="str">
+        <v>ZUM2Z</v>
+      </c>
+      <c r="D58" t="str">
+        <v>2025-06-17</v>
+      </c>
+      <c r="E58" t="str">
+        <v>18</v>
+      </c>
+      <c r="F58" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G58" t="str">
+        <v>100</v>
+      </c>
+      <c r="H58" t="str">
+        <v>6.51</v>
+      </c>
+      <c r="I58" t="str">
+        <v>0</v>
+      </c>
+      <c r="J58" t="str">
+        <v>15</v>
+      </c>
+      <c r="K58" t="str">
+        <v>15.0</v>
+      </c>
+      <c r="L58" t="str">
+        <v>teste de lançamento</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B59" t="str">
+        <v>18/06/2025, 01:40</v>
+      </c>
+      <c r="C59" t="str">
+        <v>46NI7</v>
+      </c>
+      <c r="D59" t="str">
+        <v>2025-06-19</v>
+      </c>
+      <c r="E59" t="str">
+        <v>18</v>
+      </c>
+      <c r="F59" t="str">
+        <v>1/2-PIVO</v>
+      </c>
+      <c r="G59" t="str">
+        <v>70</v>
+      </c>
+      <c r="H59" t="str">
+        <v>9.30</v>
+      </c>
+      <c r="I59" t="str">
+        <v>15</v>
+      </c>
+      <c r="J59" t="str">
+        <v>28</v>
+      </c>
+      <c r="K59" t="str">
+        <v>13.0</v>
+      </c>
+      <c r="L59" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B60" t="str">
+        <v>18/06/2025, 01:41</v>
+      </c>
+      <c r="C60" t="str">
+        <v>XCIP7</v>
+      </c>
+      <c r="D60" t="str">
+        <v>2025-06-25</v>
+      </c>
+      <c r="E60" t="str">
+        <v>25</v>
+      </c>
+      <c r="F60" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G60" t="str">
+        <v>100</v>
+      </c>
+      <c r="H60" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I60" t="str">
+        <v>500</v>
+      </c>
+      <c r="J60" t="str">
+        <v>515</v>
+      </c>
+      <c r="K60" t="str">
+        <v>15.0</v>
+      </c>
+      <c r="L60" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B61" t="str">
+        <v>18/06/2025, 01:42</v>
+      </c>
+      <c r="C61" t="str">
+        <v>HR3UE</v>
+      </c>
+      <c r="D61" t="str">
+        <v>2025-06-19</v>
+      </c>
+      <c r="E61" t="str">
+        <v>25</v>
+      </c>
+      <c r="F61" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G61" t="str">
+        <v>100</v>
+      </c>
+      <c r="H61" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I61" t="str">
+        <v>515</v>
+      </c>
+      <c r="J61" t="str">
+        <v>530</v>
+      </c>
+      <c r="K61" t="str">
+        <v>15.0</v>
+      </c>
+      <c r="L61" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B62" t="str">
+        <v>18/06/2025, 01:42</v>
+      </c>
+      <c r="C62" t="str">
+        <v>973XR</v>
+      </c>
+      <c r="D62" t="str">
+        <v>2025-06-25</v>
+      </c>
+      <c r="E62" t="str">
+        <v>25</v>
+      </c>
+      <c r="F62" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G62" t="str">
+        <v>100</v>
+      </c>
+      <c r="H62" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I62" t="str">
+        <v>530</v>
+      </c>
+      <c r="J62" t="str">
+        <v>545</v>
+      </c>
+      <c r="K62" t="str">
+        <v>15.0</v>
+      </c>
+      <c r="L62" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B63" t="str">
+        <v>18/06/2025, 01:43</v>
+      </c>
+      <c r="C63" t="str">
+        <v>E99VT</v>
+      </c>
+      <c r="D63" t="str">
+        <v>2025-06-19</v>
+      </c>
+      <c r="E63" t="str">
+        <v>18</v>
+      </c>
+      <c r="F63" t="str">
+        <v>ABCD</v>
+      </c>
+      <c r="G63" t="str">
+        <v>100</v>
+      </c>
+      <c r="H63" t="str">
+        <v>6.51</v>
+      </c>
+      <c r="I63" t="str">
+        <v>28</v>
+      </c>
+      <c r="J63" t="str">
+        <v>45</v>
+      </c>
+      <c r="K63" t="str">
+        <v>17.0</v>
+      </c>
+      <c r="L63" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B64" t="str">
+        <v>18/06/2025, 02:03</v>
+      </c>
+      <c r="C64" t="str">
+        <v>YKN4R</v>
+      </c>
+      <c r="D64" t="str">
+        <v>2025-06-20</v>
+      </c>
+      <c r="E64" t="str">
+        <v>133</v>
+      </c>
+      <c r="F64" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G64" t="str">
+        <v>50</v>
+      </c>
+      <c r="H64" t="str">
+        <v>10.30</v>
+      </c>
+      <c r="I64" t="str">
+        <v>0</v>
+      </c>
+      <c r="J64" t="str">
+        <v>30</v>
+      </c>
+      <c r="K64" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="L64" t="str">
+        <v>Kálito wilk vieira da silva</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B65" t="str">
+        <v>18/06/2025, 02:05</v>
+      </c>
+      <c r="C65" t="str">
+        <v>VJSAL</v>
+      </c>
+      <c r="D65" t="str">
+        <v>2025-06-25</v>
+      </c>
+      <c r="E65" t="str">
+        <v>133</v>
+      </c>
+      <c r="F65" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G65" t="str">
+        <v>50</v>
+      </c>
+      <c r="H65" t="str">
+        <v>10.30</v>
+      </c>
+      <c r="I65" t="str">
+        <v>0</v>
+      </c>
+      <c r="J65" t="str">
+        <v>30</v>
+      </c>
+      <c r="K65" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="L65" t="str">
+        <v>segundo teste de lançamento por Kálito Wilk</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B66" t="str">
+        <v>18/06/2025, 02:15</v>
+      </c>
+      <c r="C66" t="str">
+        <v>44LQ9</v>
+      </c>
+      <c r="D66" t="str">
+        <v>2025-06-18</v>
+      </c>
+      <c r="E66" t="str">
+        <v>25</v>
+      </c>
+      <c r="F66" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G66" t="str">
+        <v>100</v>
+      </c>
+      <c r="H66" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I66" t="str">
+        <v>545</v>
+      </c>
+      <c r="J66" t="str">
+        <v>560</v>
+      </c>
+      <c r="K66" t="str">
+        <v>15.0</v>
+      </c>
+      <c r="L66" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B67" t="str">
+        <v>18/06/2025, 02:15</v>
+      </c>
+      <c r="C67" t="str">
+        <v>6G4FH</v>
+      </c>
+      <c r="D67" t="str">
+        <v>2025-06-17</v>
+      </c>
+      <c r="E67" t="str">
+        <v>25</v>
+      </c>
+      <c r="F67" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G67" t="str">
+        <v>100</v>
+      </c>
+      <c r="H67" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I67" t="str">
+        <v>560</v>
+      </c>
+      <c r="J67" t="str">
+        <v>575</v>
+      </c>
+      <c r="K67" t="str">
+        <v>15.0</v>
+      </c>
+      <c r="L67" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B68" t="str">
+        <v>18/06/2025, 02:16</v>
+      </c>
+      <c r="C68" t="str">
+        <v>GN18D</v>
+      </c>
+      <c r="D68" t="str">
+        <v>2025-06-25</v>
+      </c>
+      <c r="E68" t="str">
+        <v>25</v>
+      </c>
+      <c r="F68" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G68" t="str">
+        <v>10</v>
+      </c>
+      <c r="H68" t="str">
+        <v>58.00</v>
+      </c>
+      <c r="I68" t="str">
+        <v>575</v>
+      </c>
+      <c r="J68" t="str">
+        <v>589</v>
+      </c>
+      <c r="K68" t="str">
+        <v>14.0</v>
+      </c>
+      <c r="L68" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B69" t="str">
+        <v>18/06/2025, 02:18</v>
+      </c>
+      <c r="C69" t="str">
+        <v>PQ5T5</v>
+      </c>
+      <c r="D69" t="str">
+        <v>2025-06-25</v>
+      </c>
+      <c r="E69" t="str">
+        <v>47</v>
+      </c>
+      <c r="F69" t="str">
+        <v>1/2-PIVO</v>
+      </c>
+      <c r="G69" t="str">
+        <v>100</v>
+      </c>
+      <c r="H69" t="str">
+        <v>7.42</v>
+      </c>
+      <c r="I69" t="str">
+        <v>15</v>
+      </c>
+      <c r="J69" t="str">
+        <v>45</v>
+      </c>
+      <c r="K69" t="str">
+        <v>30.0</v>
+      </c>
+      <c r="L69" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B70" t="str">
+        <v>18/06/2025, 02:21</v>
+      </c>
+      <c r="C70" t="str">
+        <v>N2BCM</v>
+      </c>
+      <c r="D70" t="str">
+        <v>2025-06-18</v>
+      </c>
+      <c r="E70" t="str">
+        <v>25</v>
+      </c>
+      <c r="F70" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G70" t="str">
+        <v>25</v>
+      </c>
+      <c r="H70" t="str">
+        <v>23.20</v>
+      </c>
+      <c r="I70" t="str">
+        <v>589</v>
+      </c>
+      <c r="J70" t="str">
+        <v>600</v>
+      </c>
+      <c r="K70" t="str">
+        <v>11.0</v>
+      </c>
+      <c r="L70" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B71" t="str">
+        <v>18/06/2025, 03:01</v>
+      </c>
+      <c r="C71" t="str">
+        <v>NGKBM</v>
+      </c>
+      <c r="D71" t="str">
+        <v>2025-06-18</v>
+      </c>
+      <c r="E71" t="str">
+        <v>25</v>
+      </c>
+      <c r="F71" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G71" t="str">
+        <v>100</v>
+      </c>
+      <c r="H71" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I71" t="str">
+        <v>600</v>
+      </c>
+      <c r="J71" t="str">
+        <v>615</v>
+      </c>
+      <c r="K71" t="str">
+        <v>15.0</v>
+      </c>
+      <c r="L71" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B72" t="str">
+        <v>18/06/2025, 03:12</v>
+      </c>
+      <c r="C72" t="str">
+        <v>HQTLM</v>
+      </c>
+      <c r="D72" t="str">
+        <v>2025-06-27</v>
+      </c>
+      <c r="E72" t="str">
+        <v>38</v>
+      </c>
+      <c r="F72" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G72" t="str">
+        <v>100</v>
+      </c>
+      <c r="H72" t="str">
+        <v>8.05</v>
+      </c>
+      <c r="I72" t="str">
+        <v>0</v>
+      </c>
+      <c r="J72" t="str">
+        <v>15</v>
+      </c>
+      <c r="K72" t="str">
+        <v>15.0</v>
+      </c>
+      <c r="L72" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B73" t="str">
+        <v>18/06/2025, 03:26</v>
+      </c>
+      <c r="C73" t="str">
+        <v>WW84J</v>
+      </c>
+      <c r="D73" t="str">
+        <v>2025-06-18</v>
+      </c>
+      <c r="E73" t="str">
+        <v>25</v>
+      </c>
+      <c r="F73" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G73" t="str">
+        <v>100</v>
+      </c>
+      <c r="H73" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I73" t="str">
+        <v>615</v>
+      </c>
+      <c r="J73" t="str">
+        <v>630</v>
+      </c>
+      <c r="K73" t="str">
+        <v>15.0</v>
+      </c>
+      <c r="L73" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B74" t="str">
+        <v>18/06/2025, 03:27</v>
+      </c>
+      <c r="C74" t="str">
+        <v>44SG8</v>
+      </c>
+      <c r="D74" t="str">
+        <v>2025-06-19</v>
+      </c>
+      <c r="E74" t="str">
+        <v>25</v>
+      </c>
+      <c r="F74" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G74" t="str">
+        <v>100</v>
+      </c>
+      <c r="H74" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I74" t="str">
+        <v>630</v>
+      </c>
+      <c r="J74" t="str">
+        <v>645</v>
+      </c>
+      <c r="K74" t="str">
+        <v>15.0</v>
+      </c>
+      <c r="L74" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B75" t="str">
+        <v>18/06/2025, 03:28</v>
+      </c>
+      <c r="C75" t="str">
+        <v>VC1GH</v>
+      </c>
+      <c r="D75" t="str">
+        <v>2025-06-17</v>
+      </c>
+      <c r="E75" t="str">
+        <v>25</v>
+      </c>
+      <c r="F75" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G75" t="str">
+        <v>100</v>
+      </c>
+      <c r="H75" t="str">
+        <v>5.80</v>
+      </c>
+      <c r="I75" t="str">
+        <v>645</v>
+      </c>
+      <c r="J75" t="str">
+        <v>660</v>
+      </c>
+      <c r="K75" t="str">
+        <v>15.0</v>
+      </c>
+      <c r="L75" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B76" t="str">
+        <v>18/06/2025, 03:29</v>
+      </c>
+      <c r="C76" t="str">
+        <v>1FX6M</v>
+      </c>
+      <c r="D76" t="str">
+        <v>2025-06-11</v>
+      </c>
+      <c r="E76" t="str">
+        <v>15</v>
+      </c>
+      <c r="F76" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G76" t="str">
+        <v>100</v>
+      </c>
+      <c r="H76" t="str">
+        <v>7.38</v>
+      </c>
+      <c r="I76" t="str">
+        <v>920</v>
+      </c>
+      <c r="J76" t="str">
+        <v>935</v>
+      </c>
+      <c r="K76" t="str">
+        <v>15.0</v>
+      </c>
+      <c r="L76" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B77" t="str">
+        <v>18/06/2025, 03:31</v>
+      </c>
+      <c r="C77" t="str">
+        <v>40LD4</v>
+      </c>
+      <c r="D77" t="str">
+        <v>2025-06-28</v>
+      </c>
+      <c r="E77" t="str">
+        <v>15</v>
+      </c>
+      <c r="F77" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G77" t="str">
+        <v>80</v>
+      </c>
+      <c r="H77" t="str">
+        <v>9.22</v>
+      </c>
+      <c r="I77" t="str">
+        <v>935</v>
+      </c>
+      <c r="J77" t="str">
+        <v>952</v>
+      </c>
+      <c r="K77" t="str">
+        <v>17.0</v>
+      </c>
+      <c r="L77" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B78" t="str">
+        <v>18/06/2025, 03:34</v>
+      </c>
+      <c r="C78" t="str">
+        <v>7SDAY</v>
+      </c>
+      <c r="D78" t="str">
+        <v>2025-06-18</v>
+      </c>
+      <c r="E78" t="str">
+        <v>74</v>
+      </c>
+      <c r="F78" t="str">
+        <v>COMPLETO</v>
+      </c>
+      <c r="G78" t="str">
+        <v>100</v>
+      </c>
+      <c r="H78" t="str">
+        <v>6.76</v>
+      </c>
+      <c r="I78" t="str">
+        <v>515</v>
+      </c>
+      <c r="J78" t="str">
+        <v>535</v>
+      </c>
+      <c r="K78" t="str">
+        <v>20.0</v>
+      </c>
+      <c r="L78" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L39"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L78"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>